<commit_message>
- renamed "R" folder to "components" - complete rewrite of functional UI tests - fixed bug that caused scalar data from local file not being loaded in certain situations
</commit_message>
<xml_diff>
--- a/tests/data/transport.xlsx
+++ b/tests/data/transport.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fproske/Documents/products/miro/tests/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBDE1AA-A5E8-504C-8AF7-02E0FCFAF5A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="5040" yWindow="3360" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="scalars" sheetId="1" r:id="rId1"/>
+    <sheet name="_scalars" sheetId="1" r:id="rId1"/>
     <sheet name="a" sheetId="2" r:id="rId2"/>
     <sheet name="b" sheetId="3" r:id="rId3"/>
     <sheet name="d" sheetId="4" r:id="rId4"/>
     <sheet name="ilocdata" sheetId="5" r:id="rId5"/>
     <sheet name="jlocdata" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -78,8 +84,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +122,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -162,7 +176,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -194,9 +208,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -228,6 +260,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -403,14 +453,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -421,7 +473,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -432,7 +484,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -440,10 +492,10 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -451,7 +503,7 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>
@@ -460,14 +512,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -475,7 +527,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -483,7 +535,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -497,14 +549,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -512,7 +564,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -520,7 +572,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -528,7 +580,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -542,14 +594,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -560,7 +612,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -571,7 +623,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -582,7 +634,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -593,7 +645,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -604,7 +656,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -615,7 +667,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -632,14 +684,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -650,7 +702,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -661,7 +713,7 @@
         <v>-122.335167</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -669,7 +721,7 @@
         <v>32.715736</v>
       </c>
       <c r="C3">
-        <v>-117.161087</v>
+        <v>-117.16108699999999</v>
       </c>
     </row>
   </sheetData>
@@ -678,14 +730,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -696,37 +748,37 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
       <c r="B2">
-        <v>40.73061</v>
+        <v>40.730609999999999</v>
       </c>
       <c r="C2">
-        <v>-73.935242</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>-73.935242000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3">
-        <v>41.881832</v>
+        <v>41.881832000000003</v>
       </c>
       <c r="C3">
-        <v>-87.623177</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>-87.623176999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4">
-        <v>39.056198</v>
+        <v>39.056198000000002</v>
       </c>
       <c r="C4">
-        <v>-95.695312</v>
+        <v>-95.695312000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>